<commit_message>
Optimized functions and re-write them into class.
</commit_message>
<xml_diff>
--- a/Test/Teacher_List.xlsx
+++ b/Test/Teacher_List.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianl\Documents\GitHub\XDF\Test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9288"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>俞文龙</t>
   </si>
@@ -193,12 +198,12 @@
     <t>李巍</t>
   </si>
   <si>
+    <t>贾诗丛</t>
+  </si>
+  <si>
     <t>安毓</t>
   </si>
   <si>
-    <t>贾诗丛</t>
-  </si>
-  <si>
     <t>吕欣桐</t>
   </si>
   <si>
@@ -512,25 +517,43 @@
   </si>
   <si>
     <t>李露阳</t>
+  </si>
+  <si>
+    <t>教师姓名</t>
+  </si>
+  <si>
+    <t>总产能</t>
+  </si>
+  <si>
+    <t>总课时</t>
+  </si>
+  <si>
+    <t>产能/课时</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -546,15 +569,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -842,1348 +874,2356 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B166"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D167"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="n">
+      <c r="B2">
         <v>1353896.22</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="C2">
+        <v>2158</v>
+      </c>
+      <c r="D2">
+        <v>627.38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>1214396.37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>1214396.3700000001</v>
+      </c>
+      <c r="C3">
+        <v>1498</v>
+      </c>
+      <c r="D3">
+        <v>810.68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B4">
         <v>1117574.74</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="C4">
+        <v>1672</v>
+      </c>
+      <c r="D4">
+        <v>668.41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>1096806.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>1096806.3999999999</v>
+      </c>
+      <c r="C5">
+        <v>1532</v>
+      </c>
+      <c r="D5">
+        <v>715.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
-        <v>1089110.84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>1089110.8400000001</v>
+      </c>
+      <c r="C6">
+        <v>1696</v>
+      </c>
+      <c r="D6">
+        <v>642.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B7">
         <v>1087591.43</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="C7">
+        <v>1722</v>
+      </c>
+      <c r="D7">
+        <v>631.59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B8">
         <v>1067865.96</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="C8">
+        <v>1223</v>
+      </c>
+      <c r="D8">
+        <v>873.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B9">
         <v>1065430.77</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="C9">
+        <v>1620</v>
+      </c>
+      <c r="D9">
+        <v>657.67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B10">
         <v>1040932.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="C10">
+        <v>1634</v>
+      </c>
+      <c r="D10">
+        <v>637.04999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
-        <v>981512.9899999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>981512.98999999987</v>
+      </c>
+      <c r="C11">
+        <v>1531</v>
+      </c>
+      <c r="D11">
+        <v>641.09</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B12">
         <v>979897.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="C12">
+        <v>1260</v>
+      </c>
+      <c r="D12">
+        <v>777.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B13">
         <v>978065</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="C13">
+        <v>1399</v>
+      </c>
+      <c r="D13">
+        <v>699.12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="n">
-        <v>976154.2700000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>976154.27000000014</v>
+      </c>
+      <c r="C14">
+        <v>1374</v>
+      </c>
+      <c r="D14">
+        <v>710.45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B15">
         <v>972900.98</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="C15">
+        <v>1439</v>
+      </c>
+      <c r="D15">
+        <v>676.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
-        <v>948166.1899999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+      <c r="B16">
+        <v>948166.19</v>
+      </c>
+      <c r="C16">
+        <v>1428</v>
+      </c>
+      <c r="D16">
+        <v>663.98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B17">
         <v>945729.34</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="C17">
+        <v>1264</v>
+      </c>
+      <c r="D17">
+        <v>748.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B18">
         <v>917071.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="C18">
+        <v>1469</v>
+      </c>
+      <c r="D18">
+        <v>624.28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B19">
         <v>911610</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="C19">
+        <v>1274</v>
+      </c>
+      <c r="D19">
+        <v>715.55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B20">
         <v>911461.95</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="C20">
+        <v>1372</v>
+      </c>
+      <c r="D20">
+        <v>664.33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B21">
         <v>895861.16</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+      <c r="C21">
+        <v>1286</v>
+      </c>
+      <c r="D21">
+        <v>696.63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B22">
         <v>893679.3</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+      <c r="C22">
+        <v>1122</v>
+      </c>
+      <c r="D22">
+        <v>796.51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B23">
         <v>891150</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+      <c r="C23">
+        <v>1186</v>
+      </c>
+      <c r="D23">
+        <v>751.39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="n">
-        <v>880825.5800000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+      <c r="B24">
+        <v>880825.58000000007</v>
+      </c>
+      <c r="C24">
+        <v>1563</v>
+      </c>
+      <c r="D24">
+        <v>563.54999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B25">
         <v>877456.24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+      <c r="C25">
+        <v>1137</v>
+      </c>
+      <c r="D25">
+        <v>771.73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B26">
         <v>872760.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="C26">
+        <v>1508</v>
+      </c>
+      <c r="D26">
+        <v>578.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B27">
         <v>866078.66</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+      <c r="C27">
+        <v>1162</v>
+      </c>
+      <c r="D27">
+        <v>745.33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B28">
         <v>861798.92</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+      <c r="C28">
+        <v>1280</v>
+      </c>
+      <c r="D28">
+        <v>673.28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B29">
         <v>857172.39</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+      <c r="C29">
+        <v>1380</v>
+      </c>
+      <c r="D29">
+        <v>621.14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="n">
-        <v>851701.3099999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
+      <c r="B30">
+        <v>851701.30999999994</v>
+      </c>
+      <c r="C30">
+        <v>1396</v>
+      </c>
+      <c r="D30">
+        <v>610.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B31">
         <v>838584.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
+      <c r="C31">
+        <v>1360</v>
+      </c>
+      <c r="D31">
+        <v>616.61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B32">
         <v>835391.52</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
+      <c r="C32">
+        <v>1477</v>
+      </c>
+      <c r="D32">
+        <v>565.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B33">
         <v>811945</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+      <c r="C33">
+        <v>1134</v>
+      </c>
+      <c r="D33">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B34">
         <v>807195.85</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
+      <c r="C34">
+        <v>1138</v>
+      </c>
+      <c r="D34">
+        <v>709.31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B35">
         <v>800420</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="C35">
+        <v>1168</v>
+      </c>
+      <c r="D35">
+        <v>685.29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B36">
         <v>790576</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
+      <c r="C36">
+        <v>1256</v>
+      </c>
+      <c r="D36">
+        <v>629.44000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B37">
         <v>786290</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
+      <c r="C37">
+        <v>1112</v>
+      </c>
+      <c r="D37">
+        <v>707.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B38">
         <v>783278.62</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
+      <c r="C38">
+        <v>1366</v>
+      </c>
+      <c r="D38">
+        <v>573.41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>37</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B39">
         <v>777350.86</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
+      <c r="C39">
+        <v>1025</v>
+      </c>
+      <c r="D39">
+        <v>758.39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B40">
         <v>766530</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
+      <c r="C40">
+        <v>1228</v>
+      </c>
+      <c r="D40">
+        <v>624.21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B41">
         <v>763693.08</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
+      <c r="C41">
+        <v>1469</v>
+      </c>
+      <c r="D41">
+        <v>519.87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>40</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B42">
         <v>761112</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
+      <c r="C42">
+        <v>1086</v>
+      </c>
+      <c r="D42">
+        <v>700.84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B43">
         <v>757157.16</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
+      <c r="C43">
+        <v>1110</v>
+      </c>
+      <c r="D43">
+        <v>682.12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>42</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B44">
         <v>754158.04</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
+      <c r="C44">
+        <v>1060</v>
+      </c>
+      <c r="D44">
+        <v>711.47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>43</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B45">
         <v>749489.9</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
+      <c r="C45">
+        <v>1080</v>
+      </c>
+      <c r="D45">
+        <v>693.97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B46">
         <v>747417.91</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
+      <c r="C46">
+        <v>1268</v>
+      </c>
+      <c r="D46">
+        <v>589.45000000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B47">
         <v>746646</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
+      <c r="C47">
+        <v>1424</v>
+      </c>
+      <c r="D47">
+        <v>524.33000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B48">
         <v>746025.6</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
+      <c r="C48">
+        <v>1237</v>
+      </c>
+      <c r="D48">
+        <v>603.09</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>47</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B49">
         <v>745573.51</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
+      <c r="C49">
+        <v>753</v>
+      </c>
+      <c r="D49">
+        <v>990.14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>48</v>
       </c>
-      <c r="B49" t="n">
-        <v>733019.3500000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
+      <c r="B50">
+        <v>733019.35000000009</v>
+      </c>
+      <c r="C50">
+        <v>476</v>
+      </c>
+      <c r="D50">
+        <v>1539.96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>49</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B51">
         <v>731639.67</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
+      <c r="C51">
+        <v>819</v>
+      </c>
+      <c r="D51">
+        <v>893.33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>50</v>
       </c>
-      <c r="B51" t="n">
-        <v>726091.0600000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
+      <c r="B52">
+        <v>726091.06</v>
+      </c>
+      <c r="C52">
+        <v>1068</v>
+      </c>
+      <c r="D52">
+        <v>679.86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>51</v>
       </c>
-      <c r="B52" t="n">
-        <v>725094.9299999999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
+      <c r="B53">
+        <v>725094.92999999993</v>
+      </c>
+      <c r="C53">
+        <v>1094</v>
+      </c>
+      <c r="D53">
+        <v>662.79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>52</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B54">
         <v>722620</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
+      <c r="C54">
+        <v>1168</v>
+      </c>
+      <c r="D54">
+        <v>618.67999999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>53</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B55">
         <v>720434.16</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
+      <c r="C55">
+        <v>1195</v>
+      </c>
+      <c r="D55">
+        <v>602.87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>54</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B56">
         <v>715265.21</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
+      <c r="C56">
+        <v>1340</v>
+      </c>
+      <c r="D56">
+        <v>533.78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>55</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B57">
         <v>713321.33</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
+      <c r="C57">
+        <v>1086</v>
+      </c>
+      <c r="D57">
+        <v>656.83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>56</v>
       </c>
-      <c r="B57" t="n">
-        <v>709434.4299999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
+      <c r="B58">
+        <v>709434.42999999993</v>
+      </c>
+      <c r="C58">
+        <v>924</v>
+      </c>
+      <c r="D58">
+        <v>767.79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>57</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B59">
         <v>708623.83</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
+      <c r="C59">
+        <v>1020</v>
+      </c>
+      <c r="D59">
+        <v>694.73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>58</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B60">
         <v>697800</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
+      <c r="C60">
+        <v>1072</v>
+      </c>
+      <c r="D60">
+        <v>650.92999999999995</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>59</v>
       </c>
-      <c r="B60" t="n">
-        <v>694320.3100000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
+      <c r="B61">
+        <v>694602.7</v>
+      </c>
+      <c r="C61">
+        <v>1046</v>
+      </c>
+      <c r="D61">
+        <v>664.06</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>60</v>
       </c>
-      <c r="B61" t="n">
-        <v>693902.7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" t="s">
+      <c r="B62">
+        <v>694320.31</v>
+      </c>
+      <c r="C62">
+        <v>1330</v>
+      </c>
+      <c r="D62">
+        <v>522.04999999999995</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>61</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B63">
         <v>693854.77</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
+      <c r="C63">
+        <v>1224</v>
+      </c>
+      <c r="D63">
+        <v>566.87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>62</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B64">
         <v>693160</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" t="s">
+      <c r="C64">
+        <v>1066</v>
+      </c>
+      <c r="D64">
+        <v>650.24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>63</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B65">
         <v>692467.5</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
+      <c r="C65">
+        <v>1278</v>
+      </c>
+      <c r="D65">
+        <v>541.84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>64</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B66">
         <v>688545</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
+      <c r="C66">
+        <v>958</v>
+      </c>
+      <c r="D66">
+        <v>718.73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>65</v>
       </c>
-      <c r="B66" t="n">
+      <c r="B67">
         <v>687840</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
+      <c r="C67">
+        <v>1236</v>
+      </c>
+      <c r="D67">
+        <v>556.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>66</v>
       </c>
-      <c r="B67" t="n">
+      <c r="B68">
         <v>682771</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
+      <c r="C68">
+        <v>1270</v>
+      </c>
+      <c r="D68">
+        <v>537.61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>67</v>
       </c>
-      <c r="B68" t="n">
-        <v>678841.6799999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
+      <c r="B69">
+        <v>678841.67999999993</v>
+      </c>
+      <c r="C69">
+        <v>1024</v>
+      </c>
+      <c r="D69">
+        <v>662.93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>68</v>
       </c>
-      <c r="B69" t="n">
+      <c r="B70">
         <v>671952</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
+      <c r="C70">
+        <v>1282</v>
+      </c>
+      <c r="D70">
+        <v>524.14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>69</v>
       </c>
-      <c r="B70" t="n">
+      <c r="B71">
         <v>657310</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" t="s">
+      <c r="C71">
+        <v>1076</v>
+      </c>
+      <c r="D71">
+        <v>610.88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>70</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B72">
         <v>654827.15</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" t="s">
+      <c r="C72">
+        <v>525</v>
+      </c>
+      <c r="D72">
+        <v>1247.29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>71</v>
       </c>
-      <c r="B72" t="n">
-        <v>654480.7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" t="s">
+      <c r="B73">
+        <v>654480.69999999995</v>
+      </c>
+      <c r="C73">
+        <v>1092</v>
+      </c>
+      <c r="D73">
+        <v>599.34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>72</v>
       </c>
-      <c r="B73" t="n">
+      <c r="B74">
         <v>653910</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" t="s">
+      <c r="C74">
+        <v>1070</v>
+      </c>
+      <c r="D74">
+        <v>611.13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>73</v>
       </c>
-      <c r="B74" t="n">
+      <c r="B75">
         <v>653135</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" t="s">
+      <c r="C75">
+        <v>706</v>
+      </c>
+      <c r="D75">
+        <v>925.12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>74</v>
       </c>
-      <c r="B75" t="n">
+      <c r="B76">
         <v>650003.9</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" t="s">
+      <c r="C76">
+        <v>993</v>
+      </c>
+      <c r="D76">
+        <v>654.59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>75</v>
       </c>
-      <c r="B76" t="n">
+      <c r="B77">
         <v>649686</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
+      <c r="C77">
+        <v>1084</v>
+      </c>
+      <c r="D77">
+        <v>599.34</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>76</v>
       </c>
-      <c r="B77" t="n">
+      <c r="B78">
         <v>649517</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" t="s">
+      <c r="C78">
+        <v>936</v>
+      </c>
+      <c r="D78">
+        <v>693.93</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>77</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B79">
         <v>643753.12</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" t="s">
+      <c r="C79">
+        <v>1082</v>
+      </c>
+      <c r="D79">
+        <v>594.97</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>78</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B80">
         <v>632820</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" t="s">
+      <c r="C80">
+        <v>954</v>
+      </c>
+      <c r="D80">
+        <v>663.33</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>79</v>
       </c>
-      <c r="B80" t="n">
+      <c r="B81">
         <v>624260.12</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
+      <c r="C81">
+        <v>1168</v>
+      </c>
+      <c r="D81">
+        <v>534.47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>80</v>
       </c>
-      <c r="B81" t="n">
-        <v>622514.7599999999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
+      <c r="B82">
+        <v>622514.75999999989</v>
+      </c>
+      <c r="C82">
+        <v>1094</v>
+      </c>
+      <c r="D82">
+        <v>569.03</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>81</v>
       </c>
-      <c r="B82" t="n">
-        <v>616272.4399999999</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
+      <c r="B83">
+        <v>616272.43999999994</v>
+      </c>
+      <c r="C83">
+        <v>577</v>
+      </c>
+      <c r="D83">
+        <v>1068.06</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>82</v>
       </c>
-      <c r="B83" t="n">
+      <c r="B84">
         <v>607060</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
+      <c r="C84">
+        <v>1070</v>
+      </c>
+      <c r="D84">
+        <v>567.35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>83</v>
       </c>
-      <c r="B84" t="n">
+      <c r="B85">
         <v>604190</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
+      <c r="C85">
+        <v>696</v>
+      </c>
+      <c r="D85">
+        <v>868.09</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>84</v>
       </c>
-      <c r="B85" t="n">
+      <c r="B86">
         <v>593957.38</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
+      <c r="C86">
+        <v>1030</v>
+      </c>
+      <c r="D86">
+        <v>576.66</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>85</v>
       </c>
-      <c r="B86" t="n">
+      <c r="B87">
         <v>589360</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" t="s">
+      <c r="C87">
+        <v>1082</v>
+      </c>
+      <c r="D87">
+        <v>544.70000000000005</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>86</v>
       </c>
-      <c r="B87" t="n">
+      <c r="B88">
         <v>585421</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" t="s">
+      <c r="C88">
+        <v>966</v>
+      </c>
+      <c r="D88">
+        <v>606.03</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="B88" t="n">
-        <v>568470.4099999999</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
+      <c r="B89">
+        <v>568470.40999999992</v>
+      </c>
+      <c r="C89">
+        <v>818</v>
+      </c>
+      <c r="D89">
+        <v>694.95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>88</v>
       </c>
-      <c r="B89" t="n">
+      <c r="B90">
         <v>559487.4</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
+      <c r="C90">
+        <v>1076</v>
+      </c>
+      <c r="D90">
+        <v>519.97</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>89</v>
       </c>
-      <c r="B90" t="n">
-        <v>550098.6699999999</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
+      <c r="B91">
+        <v>550098.66999999993</v>
+      </c>
+      <c r="C91">
+        <v>747</v>
+      </c>
+      <c r="D91">
+        <v>736.41</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B91" t="n">
+      <c r="B92">
         <v>547176</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
+      <c r="C92">
+        <v>878</v>
+      </c>
+      <c r="D92">
+        <v>623.21</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>91</v>
       </c>
-      <c r="B92" t="n">
+      <c r="B93">
         <v>545259.38</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
+      <c r="C93">
+        <v>1068</v>
+      </c>
+      <c r="D93">
+        <v>510.54</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>92</v>
       </c>
-      <c r="B93" t="n">
+      <c r="B94">
         <v>534294.14</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
+      <c r="C94">
+        <v>623</v>
+      </c>
+      <c r="D94">
+        <v>857.61</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>93</v>
       </c>
-      <c r="B94" t="n">
+      <c r="B95">
         <v>520120</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" t="s">
+      <c r="C95">
+        <v>858</v>
+      </c>
+      <c r="D95">
+        <v>606.20000000000005</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>94</v>
       </c>
-      <c r="B95" t="n">
+      <c r="B96">
         <v>516641.8</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
+      <c r="C96">
+        <v>928</v>
+      </c>
+      <c r="D96">
+        <v>556.73</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>95</v>
       </c>
-      <c r="B96" t="n">
+      <c r="B97">
         <v>512399</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" t="s">
+      <c r="C97">
+        <v>750</v>
+      </c>
+      <c r="D97">
+        <v>683.2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>96</v>
       </c>
-      <c r="B97" t="n">
+      <c r="B98">
         <v>511128.23</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" t="s">
+      <c r="C98">
+        <v>778</v>
+      </c>
+      <c r="D98">
+        <v>656.98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>97</v>
       </c>
-      <c r="B98" t="n">
+      <c r="B99">
         <v>505260</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" t="s">
+      <c r="C99">
+        <v>734</v>
+      </c>
+      <c r="D99">
+        <v>688.37</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>98</v>
       </c>
-      <c r="B99" t="n">
+      <c r="B100">
         <v>501048.99</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" t="s">
+      <c r="C100">
+        <v>582</v>
+      </c>
+      <c r="D100">
+        <v>860.91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>99</v>
       </c>
-      <c r="B100" t="n">
+      <c r="B101">
         <v>500953</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" t="s">
+      <c r="C101">
+        <v>842</v>
+      </c>
+      <c r="D101">
+        <v>594.96</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>100</v>
       </c>
-      <c r="B101" t="n">
+      <c r="B102">
         <v>495901.33</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" t="s">
+      <c r="C102">
+        <v>728</v>
+      </c>
+      <c r="D102">
+        <v>681.18</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>101</v>
       </c>
-      <c r="B102" t="n">
+      <c r="B103">
         <v>478142.6</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" t="s">
+      <c r="C103">
+        <v>762</v>
+      </c>
+      <c r="D103">
+        <v>627.48</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>102</v>
       </c>
-      <c r="B103" t="n">
+      <c r="B104">
         <v>442080.7</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" t="s">
+      <c r="C104">
+        <v>1006</v>
+      </c>
+      <c r="D104">
+        <v>439.44</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>103</v>
       </c>
-      <c r="B104" t="n">
+      <c r="B105">
         <v>404276.63</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" t="s">
+      <c r="C105">
+        <v>786</v>
+      </c>
+      <c r="D105">
+        <v>514.35</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>104</v>
       </c>
-      <c r="B105" t="n">
+      <c r="B106">
         <v>396800</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" t="s">
+      <c r="C106">
+        <v>890</v>
+      </c>
+      <c r="D106">
+        <v>445.84</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>105</v>
       </c>
-      <c r="B106" t="n">
+      <c r="B107">
         <v>393268.27</v>
       </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" t="s">
+      <c r="C107">
+        <v>414</v>
+      </c>
+      <c r="D107">
+        <v>949.92</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>106</v>
       </c>
-      <c r="B107" t="n">
+      <c r="B108">
         <v>389560</v>
       </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" t="s">
+      <c r="C108">
+        <v>702</v>
+      </c>
+      <c r="D108">
+        <v>554.92999999999995</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>107</v>
       </c>
-      <c r="B108" t="n">
+      <c r="B109">
         <v>380348.7</v>
       </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" t="s">
+      <c r="C109">
+        <v>668</v>
+      </c>
+      <c r="D109">
+        <v>569.38</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>108</v>
       </c>
-      <c r="B109" t="n">
+      <c r="B110">
         <v>376876.69</v>
       </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" t="s">
+      <c r="C110">
+        <v>440</v>
+      </c>
+      <c r="D110">
+        <v>856.54</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>109</v>
       </c>
-      <c r="B110" t="n">
+      <c r="B111">
         <v>373460</v>
       </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" t="s">
+      <c r="C111">
+        <v>820</v>
+      </c>
+      <c r="D111">
+        <v>455.44</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>110</v>
       </c>
-      <c r="B111" t="n">
+      <c r="B112">
         <v>365056</v>
       </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" t="s">
+      <c r="C112">
+        <v>700</v>
+      </c>
+      <c r="D112">
+        <v>521.51</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>111</v>
       </c>
-      <c r="B112" t="n">
+      <c r="B113">
         <v>358525.27</v>
       </c>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113" t="s">
+      <c r="C113">
+        <v>460</v>
+      </c>
+      <c r="D113">
+        <v>779.4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>112</v>
       </c>
-      <c r="B113" t="n">
+      <c r="B114">
         <v>357900</v>
       </c>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" t="s">
+      <c r="C114">
+        <v>822</v>
+      </c>
+      <c r="D114">
+        <v>435.4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>113</v>
       </c>
-      <c r="B114" t="n">
+      <c r="B115">
         <v>347081.96</v>
       </c>
-    </row>
-    <row r="115" spans="1:2">
-      <c r="A115" t="s">
+      <c r="C115">
+        <v>454</v>
+      </c>
+      <c r="D115">
+        <v>764.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>114</v>
       </c>
-      <c r="B115" t="n">
+      <c r="B116">
         <v>345200</v>
       </c>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116" t="s">
+      <c r="C116">
+        <v>802</v>
+      </c>
+      <c r="D116">
+        <v>430.42</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>115</v>
       </c>
-      <c r="B116" t="n">
+      <c r="B117">
         <v>342540</v>
       </c>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="A117" t="s">
+      <c r="C117">
+        <v>396</v>
+      </c>
+      <c r="D117">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>116</v>
       </c>
-      <c r="B117" t="n">
+      <c r="B118">
         <v>340741.35</v>
       </c>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" t="s">
+      <c r="C118">
+        <v>556</v>
+      </c>
+      <c r="D118">
+        <v>612.84</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>117</v>
       </c>
-      <c r="B118" t="n">
+      <c r="B119">
         <v>340408.63</v>
       </c>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" t="s">
+      <c r="C119">
+        <v>433</v>
+      </c>
+      <c r="D119">
+        <v>786.16</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>118</v>
       </c>
-      <c r="B119" t="n">
+      <c r="B120">
         <v>336940</v>
       </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" t="s">
+      <c r="C120">
+        <v>662</v>
+      </c>
+      <c r="D120">
+        <v>508.97</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>119</v>
       </c>
-      <c r="B120" t="n">
+      <c r="B121">
         <v>316100</v>
       </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" t="s">
+      <c r="C121">
+        <v>720</v>
+      </c>
+      <c r="D121">
+        <v>439.03</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>120</v>
       </c>
-      <c r="B121" t="n">
+      <c r="B122">
         <v>309240</v>
       </c>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122" t="s">
+      <c r="C122">
+        <v>754</v>
+      </c>
+      <c r="D122">
+        <v>410.13</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>121</v>
       </c>
-      <c r="B122" t="n">
+      <c r="B123">
         <v>284150.98</v>
       </c>
-    </row>
-    <row r="123" spans="1:2">
-      <c r="A123" t="s">
+      <c r="C123">
+        <v>262</v>
+      </c>
+      <c r="D123">
+        <v>1084.55</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>122</v>
       </c>
-      <c r="B123" t="n">
+      <c r="B124">
         <v>270757.39</v>
       </c>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124" t="s">
+      <c r="C124">
+        <v>426</v>
+      </c>
+      <c r="D124">
+        <v>635.58000000000004</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>123</v>
       </c>
-      <c r="B124" t="n">
+      <c r="B125">
         <v>262760</v>
       </c>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="A125" t="s">
+      <c r="C125">
+        <v>636</v>
+      </c>
+      <c r="D125">
+        <v>413.14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>124</v>
       </c>
-      <c r="B125" t="n">
+      <c r="B126">
         <v>250337</v>
       </c>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="A126" t="s">
+      <c r="C126">
+        <v>428</v>
+      </c>
+      <c r="D126">
+        <v>584.9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>125</v>
       </c>
-      <c r="B126" t="n">
+      <c r="B127">
         <v>233078</v>
       </c>
-    </row>
-    <row r="127" spans="1:2">
-      <c r="A127" t="s">
+      <c r="C127">
+        <v>428</v>
+      </c>
+      <c r="D127">
+        <v>544.57000000000005</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>126</v>
       </c>
-      <c r="B127" t="n">
+      <c r="B128">
         <v>223423.89</v>
       </c>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="A128" t="s">
+      <c r="C128">
+        <v>358</v>
+      </c>
+      <c r="D128">
+        <v>624.09</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>127</v>
       </c>
-      <c r="B128" t="n">
+      <c r="B129">
         <v>219757.6</v>
       </c>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" t="s">
+      <c r="C129">
+        <v>358</v>
+      </c>
+      <c r="D129">
+        <v>613.85</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>128</v>
       </c>
-      <c r="B129" t="n">
+      <c r="B130">
         <v>219510.17</v>
       </c>
-    </row>
-    <row r="130" spans="1:2">
-      <c r="A130" t="s">
+      <c r="C130">
+        <v>346</v>
+      </c>
+      <c r="D130">
+        <v>634.41999999999996</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>129</v>
       </c>
-      <c r="B130" t="n">
+      <c r="B131">
         <v>217648</v>
       </c>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131" t="s">
+      <c r="C131">
+        <v>262</v>
+      </c>
+      <c r="D131">
+        <v>830.72</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>130</v>
       </c>
-      <c r="B131" t="n">
+      <c r="B132">
         <v>214547.41</v>
       </c>
-    </row>
-    <row r="132" spans="1:2">
-      <c r="A132" t="s">
+      <c r="C132">
+        <v>180</v>
+      </c>
+      <c r="D132">
+        <v>1191.93</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>131</v>
       </c>
-      <c r="B132" t="n">
+      <c r="B133">
         <v>203500</v>
       </c>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" t="s">
+      <c r="C133">
+        <v>360</v>
+      </c>
+      <c r="D133">
+        <v>565.28</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>132</v>
       </c>
-      <c r="B133" t="n">
+      <c r="B134">
         <v>203156</v>
       </c>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134" t="s">
+      <c r="C134">
+        <v>366</v>
+      </c>
+      <c r="D134">
+        <v>555.07000000000005</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>133</v>
       </c>
-      <c r="B134" t="n">
+      <c r="B135">
         <v>200367.2</v>
       </c>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" t="s">
+      <c r="C135">
+        <v>354</v>
+      </c>
+      <c r="D135">
+        <v>566.01</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>134</v>
       </c>
-      <c r="B135" t="n">
+      <c r="B136">
         <v>194260</v>
       </c>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136" t="s">
+      <c r="C136">
+        <v>304</v>
+      </c>
+      <c r="D136">
+        <v>639.01</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>135</v>
       </c>
-      <c r="B136" t="n">
+      <c r="B137">
         <v>193800</v>
       </c>
-    </row>
-    <row r="137" spans="1:2">
-      <c r="A137" t="s">
+      <c r="C137">
+        <v>180</v>
+      </c>
+      <c r="D137">
+        <v>1076.67</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>136</v>
       </c>
-      <c r="B137" t="n">
+      <c r="B138">
         <v>187030</v>
       </c>
-    </row>
-    <row r="138" spans="1:2">
-      <c r="A138" t="s">
+      <c r="C138">
+        <v>398</v>
+      </c>
+      <c r="D138">
+        <v>469.92</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>137</v>
       </c>
-      <c r="B138" t="n">
+      <c r="B139">
         <v>172505</v>
       </c>
-    </row>
-    <row r="139" spans="1:2">
-      <c r="A139" t="s">
+      <c r="C139">
+        <v>228</v>
+      </c>
+      <c r="D139">
+        <v>756.6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>138</v>
       </c>
-      <c r="B139" t="n">
+      <c r="B140">
         <v>145380</v>
       </c>
-    </row>
-    <row r="140" spans="1:2">
-      <c r="A140" t="s">
+      <c r="C140">
+        <v>218</v>
+      </c>
+      <c r="D140">
+        <v>666.88</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>139</v>
       </c>
-      <c r="B140" t="n">
+      <c r="B141">
         <v>139988.96</v>
       </c>
-    </row>
-    <row r="141" spans="1:2">
-      <c r="A141" t="s">
+      <c r="C141">
+        <v>296</v>
+      </c>
+      <c r="D141">
+        <v>472.94</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>140</v>
       </c>
-      <c r="B141" t="n">
+      <c r="B142">
         <v>139920</v>
       </c>
-    </row>
-    <row r="142" spans="1:2">
-      <c r="A142" t="s">
+      <c r="C142">
+        <v>168</v>
+      </c>
+      <c r="D142">
+        <v>832.86</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>141</v>
       </c>
-      <c r="B142" t="n">
+      <c r="B143">
         <v>127101.04</v>
       </c>
-    </row>
-    <row r="143" spans="1:2">
-      <c r="A143" t="s">
+      <c r="C143">
+        <v>202</v>
+      </c>
+      <c r="D143">
+        <v>629.21</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>142</v>
       </c>
-      <c r="B143" t="n">
+      <c r="B144">
         <v>126700</v>
       </c>
-    </row>
-    <row r="144" spans="1:2">
-      <c r="A144" t="s">
+      <c r="C144">
+        <v>146</v>
+      </c>
+      <c r="D144">
+        <v>867.81</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>143</v>
       </c>
-      <c r="B144" t="n">
+      <c r="B145">
         <v>126601.4</v>
       </c>
-    </row>
-    <row r="145" spans="1:2">
-      <c r="A145" t="s">
+      <c r="C145">
+        <v>230</v>
+      </c>
+      <c r="D145">
+        <v>550.44000000000005</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>144</v>
       </c>
-      <c r="B145" t="n">
+      <c r="B146">
         <v>105660</v>
       </c>
-    </row>
-    <row r="146" spans="1:2">
-      <c r="A146" t="s">
+      <c r="C146">
+        <v>148</v>
+      </c>
+      <c r="D146">
+        <v>713.92</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>145</v>
       </c>
-      <c r="B146" t="n">
+      <c r="B147">
         <v>96920</v>
       </c>
-    </row>
-    <row r="147" spans="1:2">
-      <c r="A147" t="s">
+      <c r="C147">
+        <v>220</v>
+      </c>
+      <c r="D147">
+        <v>440.55</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>146</v>
       </c>
-      <c r="B147" t="n">
+      <c r="B148">
         <v>88979</v>
       </c>
-    </row>
-    <row r="148" spans="1:2">
-      <c r="A148" t="s">
+      <c r="C148">
+        <v>148</v>
+      </c>
+      <c r="D148">
+        <v>601.21</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>147</v>
       </c>
-      <c r="B148" t="n">
+      <c r="B149">
         <v>87658.27</v>
       </c>
-    </row>
-    <row r="149" spans="1:2">
-      <c r="A149" t="s">
+      <c r="C149">
+        <v>80</v>
+      </c>
+      <c r="D149">
+        <v>1095.73</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>148</v>
       </c>
-      <c r="B149" t="n">
+      <c r="B150">
         <v>87084.56</v>
       </c>
-    </row>
-    <row r="150" spans="1:2">
-      <c r="A150" t="s">
+      <c r="C150">
+        <v>134</v>
+      </c>
+      <c r="D150">
+        <v>649.88</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>149</v>
       </c>
-      <c r="B150" t="n">
+      <c r="B151">
         <v>83040</v>
       </c>
-    </row>
-    <row r="151" spans="1:2">
-      <c r="A151" t="s">
+      <c r="C151">
+        <v>112</v>
+      </c>
+      <c r="D151">
+        <v>741.43</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>150</v>
       </c>
-      <c r="B151" t="n">
+      <c r="B152">
         <v>70040</v>
       </c>
-    </row>
-    <row r="152" spans="1:2">
-      <c r="A152" t="s">
+      <c r="C152">
+        <v>132</v>
+      </c>
+      <c r="D152">
+        <v>530.61</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>151</v>
       </c>
-      <c r="B152" t="n">
+      <c r="B153">
         <v>63160</v>
       </c>
-    </row>
-    <row r="153" spans="1:2">
-      <c r="A153" t="s">
+      <c r="C153">
+        <v>88</v>
+      </c>
+      <c r="D153">
+        <v>717.73</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>152</v>
       </c>
-      <c r="B153" t="n">
+      <c r="B154">
         <v>51200</v>
       </c>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" t="s">
+      <c r="C154">
+        <v>132</v>
+      </c>
+      <c r="D154">
+        <v>387.88</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>153</v>
       </c>
-      <c r="B154" t="n">
+      <c r="B155">
         <v>49000</v>
       </c>
-    </row>
-    <row r="155" spans="1:2">
-      <c r="A155" t="s">
+      <c r="C155">
+        <v>132</v>
+      </c>
+      <c r="D155">
+        <v>371.21</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>154</v>
       </c>
-      <c r="B155" t="n">
+      <c r="B156">
         <v>44250</v>
       </c>
-    </row>
-    <row r="156" spans="1:2">
-      <c r="A156" t="s">
+      <c r="C156">
+        <v>110</v>
+      </c>
+      <c r="D156">
+        <v>402.27</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>155</v>
       </c>
-      <c r="B156" t="n">
+      <c r="B157">
         <v>34420</v>
       </c>
-    </row>
-    <row r="157" spans="1:2">
-      <c r="A157" t="s">
+      <c r="C157">
+        <v>80</v>
+      </c>
+      <c r="D157">
+        <v>430.25</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>156</v>
       </c>
-      <c r="B157" t="n">
+      <c r="B158">
         <v>33200</v>
       </c>
-    </row>
-    <row r="158" spans="1:2">
-      <c r="A158" t="s">
+      <c r="C158">
+        <v>86</v>
+      </c>
+      <c r="D158">
+        <v>386.05</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>157</v>
       </c>
-      <c r="B158" t="n">
+      <c r="B159">
         <v>26880</v>
       </c>
-    </row>
-    <row r="159" spans="1:2">
-      <c r="A159" t="s">
+      <c r="C159">
+        <v>46</v>
+      </c>
+      <c r="D159">
+        <v>584.35</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>158</v>
       </c>
-      <c r="B159" t="n">
+      <c r="B160">
         <v>22400</v>
       </c>
-    </row>
-    <row r="160" spans="1:2">
-      <c r="A160" t="s">
+      <c r="C160">
+        <v>64</v>
+      </c>
+      <c r="D160">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>159</v>
       </c>
-      <c r="B160" t="n">
+      <c r="B161">
         <v>21840</v>
       </c>
-    </row>
-    <row r="161" spans="1:2">
-      <c r="A161" t="s">
+      <c r="C161">
+        <v>32</v>
+      </c>
+      <c r="D161">
+        <v>682.5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>160</v>
       </c>
-      <c r="B161" t="n">
+      <c r="B162">
         <v>16900</v>
       </c>
-    </row>
-    <row r="162" spans="1:2">
-      <c r="A162" t="s">
+      <c r="C162">
+        <v>46</v>
+      </c>
+      <c r="D162">
+        <v>367.39</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>161</v>
       </c>
-      <c r="B162" t="n">
+      <c r="B163">
         <v>16100</v>
       </c>
-    </row>
-    <row r="163" spans="1:2">
-      <c r="A163" t="s">
+      <c r="C163">
+        <v>26</v>
+      </c>
+      <c r="D163">
+        <v>619.23</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>162</v>
       </c>
-      <c r="B163" t="n">
+      <c r="B164">
         <v>12078</v>
       </c>
-    </row>
-    <row r="164" spans="1:2">
-      <c r="A164" t="s">
+      <c r="C164">
+        <v>50</v>
+      </c>
+      <c r="D164">
+        <v>241.56</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>163</v>
       </c>
-      <c r="B164" t="n">
+      <c r="B165">
         <v>7320</v>
       </c>
-    </row>
-    <row r="165" spans="1:2">
-      <c r="A165" t="s">
+      <c r="C165">
+        <v>20</v>
+      </c>
+      <c r="D165">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>164</v>
       </c>
-      <c r="B165" t="n">
+      <c r="B166">
         <v>4000</v>
       </c>
-    </row>
-    <row r="166" spans="1:2">
-      <c r="A166" t="s">
+      <c r="C166">
+        <v>8</v>
+      </c>
+      <c r="D166">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>165</v>
       </c>
-      <c r="B166" t="n">
+      <c r="B167">
         <v>2100</v>
       </c>
+      <c r="C167">
+        <v>6</v>
+      </c>
+      <c r="D167">
+        <v>350</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>